<commit_message>
added logging and error handling, added bruto/neto column
</commit_message>
<xml_diff>
--- a/files/sistat_gross_net_pay_monthly.xlsx
+++ b/files/sistat_gross_net_pay_monthly.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Bruto plača Plača za mesec (EUR)</t>
+          <t>LETO</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Neto plača Plača za mesec (EUR)</t>
+          <t>Bruto/Neto</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>LETO</t>
+          <t>Plača za mesec (EUR)</t>
         </is>
       </c>
     </row>
@@ -473,17 +473,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>2134.80</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1393.86</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -500,17 +500,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>2118.46</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1384.17</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -527,17 +527,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>2181.48</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1418.90</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -554,17 +554,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>2200.58</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1430.84</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -581,17 +581,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>2209.29</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1436.65</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -608,17 +608,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>2250.67</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1463.74</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -635,17 +635,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>2219.02</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1441.51</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -662,17 +662,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>2224.26</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1445.63</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -689,17 +689,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>2207.40</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1438.67</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>2236.22</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1452.97</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -743,17 +743,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>2372.76</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1550.15</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -770,17 +770,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>2699.04</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1780.94</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -797,17 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>2306.22</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1470.56</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -824,17 +824,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>2279.85</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1453.11</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -851,17 +851,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>2312.74</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1469.77</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -878,17 +878,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>2343.89</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1487.66</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -905,17 +905,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>2342.28</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1486.88</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -932,17 +932,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>2366.79</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>1501.97</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -959,17 +959,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>2379.68</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>1508.84</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -986,17 +986,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>2353.76</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>1495.23</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>2343.07</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>1487.43</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1040,17 +1040,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>2388.35</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>1514.49</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1067,17 +1067,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>2518.74</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>1610.87</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1094,17 +1094,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>2803.97</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>1825.75</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1121,17 +1121,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>2464.35</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1569.12</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1148,17 +1148,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>2430.99</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>1550.03</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1175,17 +1175,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>2496.61</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>1580.84</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>2521.21</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>1600.77</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>2423.28</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>1571.45</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1256,17 +1256,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>2369.32</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>1542.07</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1283,17 +1283,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>2405.77</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>1562.26</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1310,17 +1310,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>2526.07</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1633.60</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1337,17 +1337,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>2513.07</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>1624.05</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>2577.71</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1665.31</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>2572.41</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>1658.13</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1418,17 +1418,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>2542.45</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>1641.31</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1445,17 +1445,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>2493.60</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>1612.51</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1472,17 +1472,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>2532.14</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>1633.23</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1499,17 +1499,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>2549.74</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>1649.32</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1526,17 +1526,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>2846.06</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>1846.60</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -1553,17 +1553,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>2572.13</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>1634.69</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1580,17 +1580,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
           <t>2505.91</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>1596.75</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1607,17 +1607,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
           <t>2542.05</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>1615.12</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1634,17 +1634,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
           <t>2580.50</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>1638.45</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1661,17 +1661,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t>2568.09</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>1629.93</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1688,17 +1688,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
           <t>2701.33</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>1707.39</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1715,17 +1715,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t>2682.05</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>1695.75</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1742,17 +1742,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>2633.81</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>1672.49</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1769,17 +1769,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
           <t>2609.04</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>1651.44</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1796,17 +1796,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>2651.65</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>1676.04</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1823,17 +1823,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>2708.27</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>1718.25</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1850,17 +1850,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>2982.28</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>1909.53</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -1877,17 +1877,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
           <t>2834.62</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>1793.17</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1904,17 +1904,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
           <t>2772.44</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>1761.17</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1931,17 +1931,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
           <t>2819.47</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>1780.07</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1958,17 +1958,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
           <t>2874.36</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>1817.56</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -1985,17 +1985,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
           <t>2004.33</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>1313.54</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2012,17 +2012,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
           <t>2004.88</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>1312.68</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2039,17 +2039,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
           <t>2080.24</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>1354.19</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2066,17 +2066,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
           <t>2054.42</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>1339.79</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2093,17 +2093,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
           <t>2072.84</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>1352.48</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2120,17 +2120,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
           <t>2103.96</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>1373.32</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2147,17 +2147,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
           <t>2060.56</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>1344.37</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
           <t>2081.69</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>1357.95</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2201,17 +2201,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
           <t>2078.17</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>1360.17</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2228,17 +2228,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
           <t>2102.55</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>1371.54</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2255,17 +2255,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
           <t>2292.68</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>1505.28</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2282,17 +2282,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
           <t>2632.33</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>1751.15</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>2023</t>
         </is>
       </c>
     </row>
@@ -2309,17 +2309,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
           <t>2185.43</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>1396.01</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
           <t>2177.25</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>1387.92</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2363,17 +2363,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
           <t>2208.91</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>1403.96</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
           <t>2236.81</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>1419.41</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2417,17 +2417,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
           <t>2240.06</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>1422.12</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2444,17 +2444,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
           <t>2214.91</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>1408.71</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2471,17 +2471,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
           <t>2242.20</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>1423.86</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2498,17 +2498,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
           <t>2226.29</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>1414.54</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2525,17 +2525,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
           <t>2221.51</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>1412.47</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2552,17 +2552,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
           <t>2268.01</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>1440.65</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2579,17 +2579,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
           <t>2431.86</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>1561.64</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2606,17 +2606,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
           <t>2721.63</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>1787.07</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>2024</t>
         </is>
       </c>
     </row>
@@ -2633,17 +2633,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
           <t>2293.72</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>1465.86</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -2660,17 +2660,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
           <t>2273.14</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>1452.42</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
           <t>2347.12</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>1488.60</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>
@@ -2714,17 +2714,2285 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Bruto</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
           <t>2357.51</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>1393.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>1384.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>1418.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>1430.84</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>1436.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>1463.74</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>1441.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>1445.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>1438.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>1452.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>1550.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>1780.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>1470.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>1453.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>1469.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>1487.66</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>1486.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>1501.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>1508.84</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1495.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>1487.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>1514.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>1610.87</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>1825.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>1569.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>1550.03</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>1580.84</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Javni in zasebni sektor - SKUPAJ</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>1600.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>1571.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>1542.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>1562.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>1633.60</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>1624.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>1665.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>1658.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>1641.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>1612.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>1633.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>1649.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>1846.60</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>1634.69</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>1596.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>1615.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>1638.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>1629.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>1707.39</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>1695.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>1672.49</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>1651.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>1676.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>1718.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>1909.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>1793.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>1761.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>1780.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Javni sektor</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>1817.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>1313.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>1312.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>1354.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>1339.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>1352.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>1373.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>1344.37</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>1357.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>1360.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>1371.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>1505.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>1751.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>1396.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>1387.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>1403.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>1419.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>1422.12</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>1408.71</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>1423.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>1414.54</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>1412.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>1440.65</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>1561.64</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>1787.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>1465.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>1452.42</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>1488.60</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Zasebni sektor</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Neto</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
         <is>
           <t>1500.27</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>2025</t>
         </is>
       </c>
     </row>

</xml_diff>